<commit_message>
SUPER DEBUG para datos del cliente
</commit_message>
<xml_diff>
--- a/inventario.xlsx
+++ b/inventario.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,546 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Frappe Moka</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" t="n">
+        <v>70</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Sin control</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Frappe Capuchino</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C3" t="n">
+        <v>70</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Sin control</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Frappe Taro</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C4" t="n">
+        <v>75</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Sin control</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Frappe Caramelo</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>75</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Sin control</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Frappe Oreo</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C6" t="n">
+        <v>80</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Sin control</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Cafe Capuchino</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C7" t="n">
+        <v>55</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Sin control</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Cafe Moka</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>60</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Sin control</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Cafe Americano</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>40</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Sin control</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Cafe Latte</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>55</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Sin control</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Latte Matcha</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C11" t="n">
+        <v>65</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Sin control</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Cold Brew</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C12" t="n">
+        <v>60</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Sin control</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Chai</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C13" t="n">
+        <v>65</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Sin control</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Caramel Macciato</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C14" t="n">
+        <v>65</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Sin control</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Latte</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C15" t="n">
+        <v>60</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Sin control</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Carterita</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>100</v>
+      </c>
+      <c r="C16" t="n">
+        <v>12</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Concha</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>100</v>
+      </c>
+      <c r="C17" t="n">
+        <v>12</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Keke</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>100</v>
+      </c>
+      <c r="C18" t="n">
+        <v>12</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Bisquete</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>100</v>
+      </c>
+      <c r="C19" t="n">
+        <v>18</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Roll de Canela</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>100</v>
+      </c>
+      <c r="C20" t="n">
+        <v>30</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Donitas</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>100</v>
+      </c>
+      <c r="C21" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Donas</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>100</v>
+      </c>
+      <c r="C22" t="n">
+        <v>15</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Waffles</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>100</v>
+      </c>
+      <c r="C23" t="n">
+        <v>65</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Sandwich</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>100</v>
+      </c>
+      <c r="C24" t="n">
+        <v>65</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Agua 500ml</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>100</v>
+      </c>
+      <c r="C25" t="n">
+        <v>13</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Coca 355ml</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>100</v>
+      </c>
+      <c r="C26" t="n">
+        <v>17</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Coca Zero 355ml</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>100</v>
+      </c>
+      <c r="C27" t="n">
+        <v>17</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Coca 600ml</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>100</v>
+      </c>
+      <c r="C28" t="n">
+        <v>25</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Coca Zero 600ml</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>100</v>
+      </c>
+      <c r="C29" t="n">
+        <v>25</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Budin</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C30" t="n">
+        <v>30</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Flan Napolitano</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C31" t="n">
+        <v>35</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Unidad</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>